<commit_message>
Still sorting out Yield Gap validation but the rest is looking good
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/CSIROobserved.xlsx
+++ b/Prototypes/Mungbean/CSIROobserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E89996-BDE1-470D-9A56-91EE228E7ADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034960C-DA15-4BBA-9CFD-248F41919E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>SimulationName</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Dalby2013_14S</t>
   </si>
   <si>
-    <t>Warra</t>
-  </si>
-  <si>
     <t>TheGlen2013_14S</t>
   </si>
   <si>
@@ -153,6 +150,15 @@
   </si>
   <si>
     <t>HarvestRipe</t>
+  </si>
+  <si>
+    <t>WarraSow2013</t>
+  </si>
+  <si>
+    <t>WarraSow2015</t>
+  </si>
+  <si>
+    <t>WarraSow2014</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -558,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -567,25 +573,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -596,7 +602,7 @@
         <v>41769</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>103</v>
@@ -628,13 +634,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5">
         <v>41873</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>98</v>
@@ -666,13 +672,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5">
         <v>41779</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
         <v>76</v>
@@ -704,13 +710,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5">
         <v>42075</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1">
         <v>83</v>
@@ -742,13 +748,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5">
         <v>42082</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1">
         <v>86</v>
@@ -780,13 +786,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5">
         <v>42106</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1">
         <v>63</v>
@@ -818,13 +824,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5">
         <v>42518</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1">
         <v>110</v>
@@ -856,13 +862,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>42480</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>97</v>
@@ -894,13 +900,13 @@
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5">
         <v>42442</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1">
         <v>91</v>
@@ -932,13 +938,13 @@
     </row>
     <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
         <v>42437</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1">
         <v>80</v>
@@ -970,13 +976,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5">
         <v>42510</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1">
         <v>96</v>
@@ -1008,13 +1014,13 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5">
         <v>42444</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1">
         <v>97</v>
@@ -1046,13 +1052,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5">
         <v>42470</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1">
         <v>96</v>
@@ -1084,13 +1090,13 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5">
         <v>42515</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1">
         <v>71</v>
@@ -1122,13 +1128,13 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="5">
         <v>42837</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1">
         <v>130</v>
@@ -1160,13 +1166,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5">
         <v>42803</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1">
         <v>70</v>
@@ -1198,13 +1204,13 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5">
         <v>42847</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1">
         <v>82</v>
@@ -1236,13 +1242,13 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5">
         <v>42917</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1">
         <v>112</v>
@@ -1274,13 +1280,13 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5">
         <v>42472</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1">
         <v>66</v>
@@ -1304,13 +1310,13 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5">
         <v>42818</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1">
         <v>90</v>
@@ -1334,13 +1340,13 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5">
         <v>42460</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1">
         <v>75</v>
@@ -1372,13 +1378,13 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="5">
         <v>42460</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1">
         <v>75</v>
@@ -1410,13 +1416,13 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5">
         <v>42460</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1">
         <v>75</v>
@@ -1448,13 +1454,13 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="5">
         <v>42460</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1">
         <v>75</v>
@@ -1486,13 +1492,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="5">
         <v>42460</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1">
         <v>75</v>
@@ -1524,13 +1530,13 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="5">
         <v>42460</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1">
         <v>75</v>
@@ -1562,13 +1568,13 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="5">
         <v>42489</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1">
         <v>113</v>
@@ -1600,13 +1606,13 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="5">
         <v>42445</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="1">
         <v>69</v>
@@ -1638,13 +1644,13 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="5">
         <v>42445</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="1">
         <v>69</v>

</xml_diff>

<commit_message>
Documented and updated as a Mungbean Model (not soybean)
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/CSIROobserved.xlsx
+++ b/Prototypes/Mungbean/CSIROobserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034960C-DA15-4BBA-9CFD-248F41919E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C149A09F-9CF8-41AB-B7F5-26CC9233010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
+    <workbookView xWindow="31950" yWindow="5625" windowWidth="20775" windowHeight="11835" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,9 @@
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>Soybean.Phenology.MaturityDAS</t>
-  </si>
-  <si>
-    <t>Soybean.AboveGround.Wt</t>
-  </si>
-  <si>
     <t>Yield</t>
   </si>
   <si>
-    <t>Soybean.Grain.HarvestIndex</t>
-  </si>
-  <si>
     <t>Dalby2013_14S</t>
   </si>
   <si>
@@ -131,24 +122,9 @@
     <t>PampasSowS6_Dec8_dens36_fallow</t>
   </si>
   <si>
-    <t>Soybean.Grain.Wt</t>
-  </si>
-  <si>
-    <t>Soybean.Phenology.CurrentStageName</t>
-  </si>
-  <si>
-    <t>Soybean.AboveGround.Wterror</t>
-  </si>
-  <si>
-    <t>Soybean.Grain.Wterror</t>
-  </si>
-  <si>
     <t>Yielderror</t>
   </si>
   <si>
-    <t>Soybean.Grain.HarvestIndexerror</t>
-  </si>
-  <si>
     <t>HarvestRipe</t>
   </si>
   <si>
@@ -159,6 +135,30 @@
   </si>
   <si>
     <t>WarraSow2014</t>
+  </si>
+  <si>
+    <t>Mungbean.Phenology.CurrentStageName</t>
+  </si>
+  <si>
+    <t>Mungbean.Phenology.MaturityDAS</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wt</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wterror</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.Wt</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.Wterror</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.HarvestIndex</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.HarvestIndexerror</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -564,45 +564,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>41769</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1">
         <v>103</v>
@@ -634,13 +634,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5">
         <v>41873</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1">
         <v>98</v>
@@ -672,13 +672,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>41779</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>76</v>
@@ -710,13 +710,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>42075</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1">
         <v>83</v>
@@ -748,13 +748,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B6" s="5">
         <v>42082</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>86</v>
@@ -786,13 +786,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>42106</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1">
         <v>63</v>
@@ -824,13 +824,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>42518</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
         <v>110</v>
@@ -862,13 +862,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>42480</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1">
         <v>97</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>42442</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1">
         <v>91</v>
@@ -938,13 +938,13 @@
     </row>
     <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5">
         <v>42437</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1">
         <v>80</v>
@@ -976,13 +976,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5">
         <v>42510</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1">
         <v>96</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5">
         <v>42444</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1">
         <v>97</v>
@@ -1052,13 +1052,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5">
         <v>42470</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1">
         <v>96</v>
@@ -1090,13 +1090,13 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5">
         <v>42515</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1">
         <v>71</v>
@@ -1128,13 +1128,13 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5">
         <v>42837</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1">
         <v>130</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5">
         <v>42803</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1">
         <v>70</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5">
         <v>42847</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1">
         <v>82</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="5">
         <v>42917</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1">
         <v>112</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5">
         <v>42472</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1">
         <v>66</v>
@@ -1310,13 +1310,13 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5">
         <v>42818</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1">
         <v>90</v>
@@ -1340,13 +1340,13 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5">
         <v>42460</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1">
         <v>75</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5">
         <v>42460</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1">
         <v>75</v>
@@ -1416,13 +1416,13 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5">
         <v>42460</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1">
         <v>75</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5">
         <v>42460</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1">
         <v>75</v>
@@ -1492,13 +1492,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" s="5">
         <v>42460</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D26" s="1">
         <v>75</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" s="5">
         <v>42460</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D27" s="1">
         <v>75</v>
@@ -1568,13 +1568,13 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5">
         <v>42489</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1">
         <v>113</v>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B29" s="5">
         <v>42445</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>69</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30" s="5">
         <v>42445</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D30" s="1">
         <v>69</v>

</xml_diff>

<commit_message>
Some points removed from dataset
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/CSIROobserved.xlsx
+++ b/Prototypes/Mungbean/CSIROobserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C149A09F-9CF8-41AB-B7F5-26CC9233010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA0B19-C430-4FE0-9419-0D4BD2D04533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="5625" windowWidth="20775" windowHeight="11835" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
+    <workbookView xWindow="28680" yWindow="5505" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -140,15 +140,6 @@
     <t>Mungbean.Phenology.CurrentStageName</t>
   </si>
   <si>
-    <t>Mungbean.Phenology.MaturityDAS</t>
-  </si>
-  <si>
-    <t>Mungbean.AboveGround.Wt</t>
-  </si>
-  <si>
-    <t>Mungbean.AboveGround.Wterror</t>
-  </si>
-  <si>
     <t>Mungbean.Grain.Wt</t>
   </si>
   <si>
@@ -159,6 +150,15 @@
   </si>
   <si>
     <t>Mungbean.Grain.HarvestIndexerror</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wtx</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wterrorx</t>
+  </si>
+  <si>
+    <t>Mungbean.Phenology.MaturityDASx</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -567,19 +567,19 @@
         <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>2</v>
@@ -588,10 +588,10 @@
         <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12">

</xml_diff>

<commit_message>
Updated with HI data
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/CSIROobserved.xlsx
+++ b/Prototypes/Mungbean/CSIROobserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA0B19-C430-4FE0-9419-0D4BD2D04533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99DF4B0-C805-470E-8264-6D9E5E5D9AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="5505" windowWidth="29040" windowHeight="15840" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{B8E29D6D-A2FA-4BA8-BDAD-B2BA57EDC6C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>SimulationName</t>
   </si>
@@ -68,21 +68,6 @@
     <t>Kingaroy</t>
   </si>
   <si>
-    <t>EmeraldSow2015_16S1</t>
-  </si>
-  <si>
-    <t>EmeraldSow2015_16S2</t>
-  </si>
-  <si>
-    <t>EmeraldSow2015_16S3</t>
-  </si>
-  <si>
-    <t>HRSSow2016_17</t>
-  </si>
-  <si>
-    <t>EmeraldSow2016_17S1</t>
-  </si>
-  <si>
     <t>EmeraldSow2016_17S2</t>
   </si>
   <si>
@@ -140,25 +125,31 @@
     <t>Mungbean.Phenology.CurrentStageName</t>
   </si>
   <si>
+    <t>Mungbean.Grain.HarvestIndex</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.HarvestIndexerror</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wtx</t>
+  </si>
+  <si>
+    <t>Mungbean.AboveGround.Wterrorx</t>
+  </si>
+  <si>
+    <t>Mungbean.Phenology.MaturityDASx</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.Total.Wt</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.Total.Wterror</t>
+  </si>
+  <si>
+    <t>Mungbean.Grain.Wterror</t>
+  </si>
+  <si>
     <t>Mungbean.Grain.Wt</t>
-  </si>
-  <si>
-    <t>Mungbean.Grain.Wterror</t>
-  </si>
-  <si>
-    <t>Mungbean.Grain.HarvestIndex</t>
-  </si>
-  <si>
-    <t>Mungbean.Grain.HarvestIndexerror</t>
-  </si>
-  <si>
-    <t>Mungbean.AboveGround.Wtx</t>
-  </si>
-  <si>
-    <t>Mungbean.AboveGround.Wterrorx</t>
-  </si>
-  <si>
-    <t>Mungbean.Phenology.MaturityDASx</t>
   </si>
 </sst>
 </file>
@@ -544,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CD354A-E582-4AF8-ABB1-6B4A2C6B68C7}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -556,7 +547,7 @@
     <col min="2" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,37 +555,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -602,7 +599,7 @@
         <v>41769</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1">
         <v>103</v>
@@ -631,16 +628,24 @@
       <c r="L2" s="7">
         <v>2.125101185498111E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <f>I2/10</f>
+        <v>78.862155999999999</v>
+      </c>
+      <c r="N2">
+        <f>J2/10</f>
+        <v>2.9572359422224257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5">
         <v>41873</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>98</v>
@@ -669,8 +674,16 @@
       <c r="L3" s="7">
         <v>4.2411664719761273E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <f t="shared" ref="M3:N25" si="0">I3/10</f>
+        <v>139.4927395</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>11.519730096183611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -678,7 +691,7 @@
         <v>41779</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
         <v>76</v>
@@ -707,8 +720,16 @@
       <c r="L4" s="7">
         <v>4.0059777201061179E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>115.10561862</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>13.167741566094895</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -716,7 +737,7 @@
         <v>42075</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1">
         <v>83</v>
@@ -745,16 +766,24 @@
       <c r="L5" s="7">
         <v>2.1841180724069157E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>79.5347186475</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>3.510750929006643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5">
         <v>42082</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1">
         <v>86</v>
@@ -783,8 +812,16 @@
       <c r="L6" s="7">
         <v>3.220960415631486E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>196.80110359999998</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>14.929338205127161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -792,7 +829,7 @@
         <v>42106</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>63</v>
@@ -821,8 +858,16 @@
       <c r="L7" s="7">
         <v>2.3347557706495849E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>66.263504273333325</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>2.8962935784988373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -830,7 +875,7 @@
         <v>42518</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>110</v>
@@ -859,8 +904,16 @@
       <c r="L8" s="7">
         <v>5.1577948334408548E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>172.29457006666664</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>20.291717113789971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -868,7 +921,7 @@
         <v>42480</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>97</v>
@@ -897,8 +950,16 @@
       <c r="L9" s="7">
         <v>9.2778191892129935E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>142.55941140000002</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>24.830288943355789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -906,7 +967,7 @@
         <v>42442</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <v>91</v>
@@ -935,16 +996,24 @@
       <c r="L10" s="7">
         <v>2.2367421943491186E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1">
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>112.05483470999999</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>9.4807853697580029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5">
         <v>42437</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
         <v>80</v>
@@ -973,8 +1042,16 @@
       <c r="L11" s="7">
         <v>6.4764546960941593E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>183.93277710000001</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>2.9508182279760105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -982,7 +1059,7 @@
         <v>42510</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
         <v>96</v>
@@ -1011,334 +1088,414 @@
       <c r="L12" s="7">
         <v>1.1422810926680875E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>147.26439899999997</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>7.8265091941149763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <v>42444</v>
+        <v>42847</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E13" s="6">
-        <v>546.86666666666667</v>
+        <v>525.16666666666663</v>
       </c>
       <c r="F13" s="6">
-        <v>65.270752340624497</v>
+        <v>12.292861523845625</v>
       </c>
       <c r="G13" s="6">
-        <v>152.73032019999997</v>
+        <v>122.65473146666666</v>
       </c>
       <c r="H13" s="6">
-        <v>9.8688474110391766</v>
+        <v>12.194592515919279</v>
       </c>
       <c r="I13" s="6">
-        <v>1527.3032020000001</v>
+        <v>1226.5473146666666</v>
       </c>
       <c r="J13" s="6">
-        <v>98.688474110391709</v>
+        <v>121.94592515919338</v>
       </c>
       <c r="K13" s="7">
-        <v>0.287590974</v>
+        <v>0.23274272100000001</v>
       </c>
       <c r="L13" s="7">
-        <v>3.9282555523223732E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>1.7857425691330499E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>122.65473146666666</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>12.194592515919338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>42470</v>
+        <v>42917</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E14" s="6">
-        <v>341.76666666666665</v>
+        <v>548.90000000000009</v>
       </c>
       <c r="F14" s="6">
-        <v>20.900505044402895</v>
+        <v>31.026816358326759</v>
       </c>
       <c r="G14" s="6">
-        <v>118.40956311333332</v>
+        <v>152.45111643333334</v>
       </c>
       <c r="H14" s="6">
-        <v>19.145040930469499</v>
+        <v>0.50618050328420561</v>
       </c>
       <c r="I14" s="6">
-        <v>1184.0956311333332</v>
+        <v>1524.5111643333332</v>
       </c>
       <c r="J14" s="6">
-        <v>191.45040930469506</v>
+        <v>5.0618050328420336</v>
       </c>
       <c r="K14" s="7">
-        <v>0.34639466399999996</v>
+        <v>0.2795663306666667</v>
       </c>
       <c r="L14" s="7">
-        <v>4.9033605022521701E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>1.6165258222426079E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>152.45111643333331</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.50618050328420339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>42515</v>
+        <v>42472</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E15" s="6">
-        <v>379.2</v>
-      </c>
-      <c r="F15" s="6">
-        <v>37.00450423034124</v>
-      </c>
+        <v>166.6</v>
+      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6">
-        <v>123.63175503333332</v>
-      </c>
-      <c r="H15" s="6">
-        <v>4.2590483981002363</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="6">
-        <v>1236.3175503333332</v>
-      </c>
-      <c r="J15" s="6">
-        <v>42.590483981002379</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="J15" s="6"/>
       <c r="K15" s="7">
-        <v>0.33500561666666667</v>
-      </c>
-      <c r="L15" s="7">
-        <v>4.6380195228279721E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.30012004799999997</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>42837</v>
+        <v>42818</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E16" s="6">
-        <v>504.5333333333333</v>
-      </c>
-      <c r="F16" s="6">
-        <v>46.040754892932839</v>
-      </c>
+        <v>172.9</v>
+      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="6">
-        <v>260.82614456666664</v>
-      </c>
-      <c r="H16" s="6">
-        <v>4.5742956705273432</v>
-      </c>
+        <v>50.4</v>
+      </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="6">
-        <v>2608.261445666667</v>
-      </c>
-      <c r="J16" s="6">
-        <v>45.74295670527345</v>
-      </c>
+        <v>504</v>
+      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="7">
-        <v>0.52443959033333332</v>
-      </c>
-      <c r="L16" s="7">
-        <v>4.1198879405919514E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.29149797599999999</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>50.4</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>42803</v>
+        <v>42460</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E17" s="6">
-        <v>442.59999999999997</v>
+        <v>347</v>
       </c>
       <c r="F17" s="6">
-        <v>41.368385674731655</v>
+        <v>53.315288614055198</v>
       </c>
       <c r="G17" s="6">
-        <v>66.218045449999991</v>
+        <v>79.87</v>
       </c>
       <c r="H17" s="6">
-        <v>10.54545848099148</v>
+        <v>12.835756048372573</v>
       </c>
       <c r="I17" s="6">
-        <v>662.1804545</v>
+        <v>798.7</v>
       </c>
       <c r="J17" s="6">
-        <v>105.45458480991452</v>
+        <v>128.35756048372565</v>
       </c>
       <c r="K17" s="7">
-        <v>0.14952263433333332</v>
+        <v>0.229874143</v>
       </c>
       <c r="L17" s="7">
-        <v>1.8598176121128147E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>8.680747437081025E-3</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>79.87</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>12.835756048372565</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>42847</v>
+        <v>42460</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E18" s="6">
-        <v>525.16666666666663</v>
+        <v>310.8</v>
       </c>
       <c r="F18" s="6">
-        <v>12.292861523845625</v>
+        <v>40.375900402756699</v>
       </c>
       <c r="G18" s="6">
-        <v>122.65473146666666</v>
+        <v>67.69</v>
       </c>
       <c r="H18" s="6">
-        <v>12.194592515919279</v>
+        <v>11.664583147288191</v>
       </c>
       <c r="I18" s="6">
-        <v>1226.5473146666666</v>
+        <v>676.90000000000009</v>
       </c>
       <c r="J18" s="6">
-        <v>121.94592515919338</v>
+        <v>116.64583147288188</v>
       </c>
       <c r="K18" s="7">
-        <v>0.23274272100000001</v>
+        <v>0.21346524550000001</v>
       </c>
       <c r="L18" s="7">
-        <v>1.7857425691330499E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>1.1467131045641656E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>67.690000000000012</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>11.664583147288187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>42917</v>
+        <v>42460</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E19" s="6">
-        <v>548.90000000000009</v>
+        <v>174.40000000000003</v>
       </c>
       <c r="F19" s="6">
-        <v>31.026816358326759</v>
+        <v>11.671046796810023</v>
       </c>
       <c r="G19" s="6">
-        <v>152.45111643333334</v>
+        <v>30.340000000000003</v>
       </c>
       <c r="H19" s="6">
-        <v>0.50618050328420561</v>
+        <v>5.2876333710523724</v>
       </c>
       <c r="I19" s="6">
-        <v>1524.5111643333332</v>
+        <v>303.40000000000003</v>
       </c>
       <c r="J19" s="6">
-        <v>5.0618050328420336</v>
+        <v>52.876333710523625</v>
       </c>
       <c r="K19" s="7">
-        <v>0.2795663306666667</v>
+        <v>0.18042612899999999</v>
       </c>
       <c r="L19" s="7">
-        <v>1.6165258222426079E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>4.0917337587205206E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>30.340000000000003</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>5.2876333710523626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>42472</v>
+        <v>42460</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E20" s="6">
-        <v>166.6</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>245.8</v>
+      </c>
+      <c r="F20" s="6">
+        <v>25.414693912511805</v>
+      </c>
       <c r="G20" s="6">
-        <v>50</v>
-      </c>
-      <c r="H20" s="6"/>
+        <v>48.87</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6.9916402462750735</v>
+      </c>
       <c r="I20" s="6">
-        <v>500</v>
-      </c>
-      <c r="J20" s="6"/>
+        <v>488.7</v>
+      </c>
+      <c r="J20" s="6">
+        <v>69.916402462750654</v>
+      </c>
       <c r="K20" s="7">
-        <v>0.30012004799999997</v>
-      </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.197356009</v>
+      </c>
+      <c r="L20" s="7">
+        <v>1.2382578503120516E-2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>48.87</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>6.9916402462750655</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>42818</v>
+        <v>42460</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E21" s="6">
-        <v>172.9</v>
-      </c>
-      <c r="F21" s="6"/>
+        <v>255</v>
+      </c>
+      <c r="F21" s="6">
+        <v>26.947108688441187</v>
+      </c>
       <c r="G21" s="6">
-        <v>50.4</v>
-      </c>
-      <c r="H21" s="6"/>
+        <v>52.7</v>
+      </c>
+      <c r="H21" s="6">
+        <v>8.2582080380673304</v>
+      </c>
       <c r="I21" s="6">
-        <v>504</v>
-      </c>
-      <c r="J21" s="6"/>
+        <v>527</v>
+      </c>
+      <c r="J21" s="6">
+        <v>82.582080380673432</v>
+      </c>
       <c r="K21" s="7">
-        <v>0.29149797599999999</v>
-      </c>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.20383851324999999</v>
+      </c>
+      <c r="L21" s="7">
+        <v>1.6160732447134969E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>52.7</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>8.2582080380673428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1346,338 +1503,180 @@
         <v>42460</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1">
         <v>75</v>
       </c>
       <c r="E22" s="6">
-        <v>347</v>
+        <v>232.79999999999998</v>
       </c>
       <c r="F22" s="6">
-        <v>53.315288614055198</v>
+        <v>25.806975801127926</v>
       </c>
       <c r="G22" s="6">
-        <v>79.87</v>
+        <v>46.97</v>
       </c>
       <c r="H22" s="6">
-        <v>12.835756048372573</v>
+        <v>7.6380167582953167</v>
       </c>
       <c r="I22" s="6">
-        <v>798.7</v>
+        <v>469.70000000000005</v>
       </c>
       <c r="J22" s="6">
-        <v>128.35756048372565</v>
+        <v>76.380167582952993</v>
       </c>
       <c r="K22" s="7">
-        <v>0.229874143</v>
+        <v>0.19876039225000003</v>
       </c>
       <c r="L22" s="7">
-        <v>8.680747437081025E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>2.0415692917228882E-2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>46.970000000000006</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>7.6380167582952989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="5">
-        <v>42460</v>
+        <v>42489</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="E23" s="6">
-        <v>310.8</v>
+        <v>434.8</v>
       </c>
       <c r="F23" s="6">
-        <v>40.375900402756699</v>
+        <v>0</v>
       </c>
       <c r="G23" s="6">
-        <v>67.69</v>
+        <v>123.8</v>
       </c>
       <c r="H23" s="6">
-        <v>11.664583147288191</v>
+        <v>0</v>
       </c>
       <c r="I23" s="6">
-        <v>676.90000000000009</v>
+        <v>1238</v>
       </c>
       <c r="J23" s="6">
-        <v>116.64583147288188</v>
+        <v>0</v>
       </c>
       <c r="K23" s="7">
-        <v>0.21346524550000001</v>
+        <v>0.28472861100000002</v>
       </c>
       <c r="L23" s="7">
-        <v>1.1467131045641656E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>123.8</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>42460</v>
+        <v>42445</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E24" s="6">
-        <v>174.40000000000003</v>
+        <v>498.32857142499995</v>
       </c>
       <c r="F24" s="6">
-        <v>11.671046796810023</v>
+        <v>58.649594170147274</v>
       </c>
       <c r="G24" s="6">
-        <v>30.340000000000003</v>
+        <v>103.757142875</v>
       </c>
       <c r="H24" s="6">
-        <v>5.2876333710523724</v>
+        <v>19.535021754916656</v>
       </c>
       <c r="I24" s="6">
-        <v>303.40000000000003</v>
+        <v>1037.57142875</v>
       </c>
       <c r="J24" s="6">
-        <v>52.876333710523625</v>
+        <v>195.35021754916676</v>
       </c>
       <c r="K24" s="7">
-        <v>0.18042612899999999</v>
+        <v>0.20248820075000001</v>
       </c>
       <c r="L24" s="7">
-        <v>4.0917337587205206E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>1.7384346082848143E-2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>103.757142875</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>19.535021754916677</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>42460</v>
+        <v>42445</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E25" s="6">
-        <v>245.8</v>
+        <v>337.49999997500004</v>
       </c>
       <c r="F25" s="6">
-        <v>25.414693912511805</v>
+        <v>53.150207501341704</v>
       </c>
       <c r="G25" s="6">
-        <v>48.87</v>
+        <v>73.000000005000004</v>
       </c>
       <c r="H25" s="6">
-        <v>6.9916402462750735</v>
+        <v>18.510798467880388</v>
       </c>
       <c r="I25" s="6">
-        <v>488.7</v>
+        <v>730.00000004999993</v>
       </c>
       <c r="J25" s="6">
-        <v>69.916402462750654</v>
+        <v>185.10798467880392</v>
       </c>
       <c r="K25" s="7">
-        <v>0.197356009</v>
+        <v>0.2067481015</v>
       </c>
       <c r="L25" s="7">
-        <v>1.2382578503120516E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="5">
-        <v>42460</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="1">
-        <v>75</v>
-      </c>
-      <c r="E26" s="6">
-        <v>255</v>
-      </c>
-      <c r="F26" s="6">
-        <v>26.947108688441187</v>
-      </c>
-      <c r="G26" s="6">
-        <v>52.7</v>
-      </c>
-      <c r="H26" s="6">
-        <v>8.2582080380673304</v>
-      </c>
-      <c r="I26" s="6">
-        <v>527</v>
-      </c>
-      <c r="J26" s="6">
-        <v>82.582080380673432</v>
-      </c>
-      <c r="K26" s="7">
-        <v>0.20383851324999999</v>
-      </c>
-      <c r="L26" s="7">
-        <v>1.6160732447134969E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5">
-        <v>42460</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1">
-        <v>75</v>
-      </c>
-      <c r="E27" s="6">
-        <v>232.79999999999998</v>
-      </c>
-      <c r="F27" s="6">
-        <v>25.806975801127926</v>
-      </c>
-      <c r="G27" s="6">
-        <v>46.97</v>
-      </c>
-      <c r="H27" s="6">
-        <v>7.6380167582953167</v>
-      </c>
-      <c r="I27" s="6">
-        <v>469.70000000000005</v>
-      </c>
-      <c r="J27" s="6">
-        <v>76.380167582952993</v>
-      </c>
-      <c r="K27" s="7">
-        <v>0.19876039225000003</v>
-      </c>
-      <c r="L27" s="7">
-        <v>2.0415692917228882E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="5">
-        <v>42489</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="1">
-        <v>113</v>
-      </c>
-      <c r="E28" s="6">
-        <v>434.8</v>
-      </c>
-      <c r="F28" s="6">
-        <v>0</v>
-      </c>
-      <c r="G28" s="6">
-        <v>123.8</v>
-      </c>
-      <c r="H28" s="6">
-        <v>0</v>
-      </c>
-      <c r="I28" s="6">
-        <v>1238</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0.28472861100000002</v>
-      </c>
-      <c r="L28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5">
-        <v>42445</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="1">
-        <v>69</v>
-      </c>
-      <c r="E29" s="6">
-        <v>498.32857142499995</v>
-      </c>
-      <c r="F29" s="6">
-        <v>58.649594170147274</v>
-      </c>
-      <c r="G29" s="6">
-        <v>103.757142875</v>
-      </c>
-      <c r="H29" s="6">
-        <v>19.535021754916656</v>
-      </c>
-      <c r="I29" s="6">
-        <v>1037.57142875</v>
-      </c>
-      <c r="J29" s="6">
-        <v>195.35021754916676</v>
-      </c>
-      <c r="K29" s="7">
-        <v>0.20248820075000001</v>
-      </c>
-      <c r="L29" s="7">
-        <v>1.7384346082848143E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5">
-        <v>42445</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="1">
-        <v>69</v>
-      </c>
-      <c r="E30" s="6">
-        <v>337.49999997500004</v>
-      </c>
-      <c r="F30" s="6">
-        <v>53.150207501341704</v>
-      </c>
-      <c r="G30" s="6">
-        <v>73.000000005000004</v>
-      </c>
-      <c r="H30" s="6">
-        <v>18.510798467880388</v>
-      </c>
-      <c r="I30" s="6">
-        <v>730.00000004999993</v>
-      </c>
-      <c r="J30" s="6">
-        <v>185.10798467880392</v>
-      </c>
-      <c r="K30" s="7">
-        <v>0.2067481015</v>
-      </c>
-      <c r="L30" s="7">
         <v>2.4225189761673854E-2</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>73.00000000499999</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>18.510798467880392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>